<commit_message>
added N/A in the co tab
</commit_message>
<xml_diff>
--- a/spec/support/validRoSpreadsheet.xlsx
+++ b/spec/support/validRoSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhaisajoness/Documents/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{406EE2D0-73BD-ED4B-B6DD-945FE20E4230}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{23C57C79-DF8D-614F-BC0D-F5BB7DCC5CD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22300" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26120" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
   <si>
     <t>Example</t>
   </si>
@@ -2365,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
@@ -3444,8 +3444,8 @@
       <c r="AJ7" s="22">
         <v>43191</v>
       </c>
-      <c r="AK7" s="22">
-        <v>43191</v>
+      <c r="AK7" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="AL7" s="22">
         <v>43191</v>
@@ -3555,7 +3555,6 @@
       <c r="AH8" s="28"/>
       <c r="AI8" s="28"/>
       <c r="AJ8" s="28"/>
-      <c r="AK8" s="28"/>
       <c r="AL8" s="28"/>
       <c r="AM8" s="28"/>
       <c r="AN8" s="28"/>
@@ -6163,7 +6162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -6274,7 +6275,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Finally tests are passing
</commit_message>
<xml_diff>
--- a/spec/support/validRoSpreadsheet.xlsx
+++ b/spec/support/validRoSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhaisajoness/Documents/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{23C57C79-DF8D-614F-BC0D-F5BB7DCC5CD6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1BCC1B81-5A2E-A542-899B-025A1D6F8F69}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26120" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26120" windowHeight="14120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="127">
   <si>
     <t>Example</t>
   </si>
@@ -2365,7 +2365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
@@ -6162,8 +6162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -6240,7 +6240,9 @@
     </row>
     <row r="8" spans="1:5" ht="17" customHeight="1">
       <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="B8" s="28" t="s">
+        <v>126</v>
+      </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>

</xml_diff>

<commit_message>
Spreadsheet Validation | co-non-availability-days (#6103)
Connects #6063

### Description
This PR validates  co non-availability days
### Acceptance Criteria 
- [ ]  When validating co non-availability days, we'll allow either a date type, or N/A
- [ ] When importing co non-availability days, we'll skip N/A
</commit_message>
<xml_diff>
--- a/spec/support/validRoSpreadsheet.xlsx
+++ b/spec/support/validRoSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhaisajoness/Documents/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{406EE2D0-73BD-ED4B-B6DD-945FE20E4230}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1BCC1B81-5A2E-A542-899B-025A1D6F8F69}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22300" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26120" windowHeight="14120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="127">
   <si>
     <t>Example</t>
   </si>
@@ -2365,8 +2365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView showGridLines="0" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
@@ -3444,8 +3444,8 @@
       <c r="AJ7" s="22">
         <v>43191</v>
       </c>
-      <c r="AK7" s="22">
-        <v>43191</v>
+      <c r="AK7" s="28" t="s">
+        <v>126</v>
       </c>
       <c r="AL7" s="22">
         <v>43191</v>
@@ -3555,7 +3555,6 @@
       <c r="AH8" s="28"/>
       <c r="AI8" s="28"/>
       <c r="AJ8" s="28"/>
-      <c r="AK8" s="28"/>
       <c r="AL8" s="28"/>
       <c r="AM8" s="28"/>
       <c r="AN8" s="28"/>
@@ -6163,7 +6162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -6239,7 +6240,9 @@
     </row>
     <row r="8" spans="1:5" ht="17" customHeight="1">
       <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="B8" s="28" t="s">
+        <v>126</v>
+      </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
@@ -6274,7 +6277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV100"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
Updated the test RO spreadsheet based on the new requirements
</commit_message>
<xml_diff>
--- a/spec/support/validRoSpreadsheet.xlsx
+++ b/spec/support/validRoSpreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomas/Desktop/tmp/compare/redone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4E0DB1-F6CA-9344-8534-13B50355BAFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF95FDD3-10D1-3749-BD00-E8A4203A0C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="800" windowWidth="37280" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="123">
   <si>
     <t>Example</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
+  </si>
+  <si>
+    <t>Number of Hearing Days Without Rooms in Date Range</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -512,7 +515,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -734,19 +737,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -942,11 +932,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1001,13 +1019,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1022,9 +1040,6 @@
     <xf numFmtId="14" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1040,25 +1055,25 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1071,10 +1086,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2269,9 +2290,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
@@ -2282,24 +2305,24 @@
     <col min="7" max="254" width="11" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="56" customHeight="1">
+    <row r="1" spans="1:57" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2345,7 +2368,7 @@
       <c r="BD1" s="4"/>
       <c r="BE1" s="5"/>
     </row>
-    <row r="2" spans="1:57" ht="39" customHeight="1">
+    <row r="2" spans="1:57" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -2518,7 +2541,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:57" ht="34" customHeight="1">
+    <row r="3" spans="1:57" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>59</v>
       </c>
@@ -2691,7 +2714,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:57" ht="32" customHeight="1">
+    <row r="4" spans="1:57" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>116</v>
       </c>
@@ -2864,7 +2887,7 @@
         <v>43114</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="17" customHeight="1">
+    <row r="5" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="20">
         <v>43497</v>
@@ -3035,7 +3058,7 @@
         <v>43115</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="17" customHeight="1">
+    <row r="6" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="23">
         <v>43540</v>
@@ -3206,7 +3229,7 @@
         <v>43225</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="17" customHeight="1">
+    <row r="7" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="24">
         <v>43576</v>
@@ -3377,7 +3400,7 @@
         <v>43191</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="17" customHeight="1">
+    <row r="8" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="26">
         <v>43604</v>
@@ -3438,7 +3461,7 @@
       <c r="BD8" s="29"/>
       <c r="BE8" s="29"/>
     </row>
-    <row r="9" spans="1:57" ht="17" customHeight="1">
+    <row r="9" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="30"/>
       <c r="C9" s="31"/>
@@ -3497,7 +3520,7 @@
       <c r="BD9" s="29"/>
       <c r="BE9" s="29"/>
     </row>
-    <row r="10" spans="1:57" ht="17" customHeight="1">
+    <row r="10" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
@@ -3556,7 +3579,7 @@
       <c r="BD10" s="28"/>
       <c r="BE10" s="28"/>
     </row>
-    <row r="11" spans="1:57" ht="17" customHeight="1">
+    <row r="11" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="34"/>
       <c r="C11" s="31"/>
@@ -3615,7 +3638,7 @@
       <c r="BD11" s="31"/>
       <c r="BE11" s="35"/>
     </row>
-    <row r="12" spans="1:57" ht="17" customHeight="1">
+    <row r="12" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
@@ -3674,7 +3697,7 @@
       <c r="BD12" s="33"/>
       <c r="BE12" s="33"/>
     </row>
-    <row r="13" spans="1:57" ht="17" customHeight="1">
+    <row r="13" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="34"/>
       <c r="C13" s="31"/>
@@ -3733,7 +3756,7 @@
       <c r="BD13" s="31"/>
       <c r="BE13" s="35"/>
     </row>
-    <row r="14" spans="1:57" ht="17" customHeight="1">
+    <row r="14" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="32"/>
       <c r="C14" s="33"/>
@@ -3792,7 +3815,7 @@
       <c r="BD14" s="33"/>
       <c r="BE14" s="33"/>
     </row>
-    <row r="15" spans="1:57" ht="17" customHeight="1">
+    <row r="15" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="34"/>
       <c r="C15" s="31"/>
@@ -3851,7 +3874,7 @@
       <c r="BD15" s="31"/>
       <c r="BE15" s="35"/>
     </row>
-    <row r="16" spans="1:57" ht="17" customHeight="1">
+    <row r="16" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
@@ -3910,7 +3933,7 @@
       <c r="BD16" s="33"/>
       <c r="BE16" s="33"/>
     </row>
-    <row r="17" spans="1:57" ht="17" customHeight="1">
+    <row r="17" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="34"/>
       <c r="C17" s="31"/>
@@ -3969,7 +3992,7 @@
       <c r="BD17" s="31"/>
       <c r="BE17" s="35"/>
     </row>
-    <row r="18" spans="1:57" ht="17" customHeight="1">
+    <row r="18" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
@@ -4028,7 +4051,7 @@
       <c r="BD18" s="33"/>
       <c r="BE18" s="33"/>
     </row>
-    <row r="19" spans="1:57" ht="17" customHeight="1">
+    <row r="19" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="34"/>
       <c r="C19" s="31"/>
@@ -4087,7 +4110,7 @@
       <c r="BD19" s="31"/>
       <c r="BE19" s="35"/>
     </row>
-    <row r="20" spans="1:57" ht="17" customHeight="1">
+    <row r="20" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="32"/>
       <c r="C20" s="33"/>
@@ -4146,7 +4169,7 @@
       <c r="BD20" s="33"/>
       <c r="BE20" s="33"/>
     </row>
-    <row r="21" spans="1:57" ht="17" customHeight="1">
+    <row r="21" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="34"/>
       <c r="C21" s="31"/>
@@ -4205,7 +4228,7 @@
       <c r="BD21" s="31"/>
       <c r="BE21" s="35"/>
     </row>
-    <row r="22" spans="1:57" ht="17" customHeight="1">
+    <row r="22" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="32"/>
       <c r="C22" s="33"/>
@@ -4264,7 +4287,7 @@
       <c r="BD22" s="33"/>
       <c r="BE22" s="33"/>
     </row>
-    <row r="23" spans="1:57" ht="17" customHeight="1">
+    <row r="23" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="34"/>
       <c r="C23" s="31"/>
@@ -4323,7 +4346,7 @@
       <c r="BD23" s="31"/>
       <c r="BE23" s="35"/>
     </row>
-    <row r="24" spans="1:57" ht="17" customHeight="1">
+    <row r="24" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
@@ -4382,7 +4405,7 @@
       <c r="BD24" s="33"/>
       <c r="BE24" s="33"/>
     </row>
-    <row r="25" spans="1:57" ht="17" customHeight="1">
+    <row r="25" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="34"/>
       <c r="C25" s="31"/>
@@ -4441,7 +4464,7 @@
       <c r="BD25" s="31"/>
       <c r="BE25" s="35"/>
     </row>
-    <row r="26" spans="1:57" ht="17" customHeight="1">
+    <row r="26" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="32"/>
       <c r="C26" s="33"/>
@@ -4500,7 +4523,7 @@
       <c r="BD26" s="33"/>
       <c r="BE26" s="33"/>
     </row>
-    <row r="27" spans="1:57" ht="17" customHeight="1">
+    <row r="27" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="34"/>
       <c r="C27" s="31"/>
@@ -4559,7 +4582,7 @@
       <c r="BD27" s="31"/>
       <c r="BE27" s="35"/>
     </row>
-    <row r="28" spans="1:57" ht="17" customHeight="1">
+    <row r="28" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -4618,7 +4641,7 @@
       <c r="BD28" s="33"/>
       <c r="BE28" s="33"/>
     </row>
-    <row r="29" spans="1:57" ht="17" customHeight="1">
+    <row r="29" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="34"/>
       <c r="C29" s="31"/>
@@ -4677,7 +4700,7 @@
       <c r="BD29" s="31"/>
       <c r="BE29" s="35"/>
     </row>
-    <row r="30" spans="1:57" ht="17" customHeight="1">
+    <row r="30" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
@@ -4736,7 +4759,7 @@
       <c r="BD30" s="33"/>
       <c r="BE30" s="33"/>
     </row>
-    <row r="31" spans="1:57" ht="17" customHeight="1">
+    <row r="31" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="34"/>
       <c r="C31" s="31"/>
@@ -4795,7 +4818,7 @@
       <c r="BD31" s="31"/>
       <c r="BE31" s="35"/>
     </row>
-    <row r="32" spans="1:57" ht="17" customHeight="1">
+    <row r="32" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="32"/>
       <c r="C32" s="33"/>
@@ -4854,7 +4877,7 @@
       <c r="BD32" s="33"/>
       <c r="BE32" s="33"/>
     </row>
-    <row r="33" spans="1:57" ht="17" customHeight="1">
+    <row r="33" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="34"/>
       <c r="C33" s="31"/>
@@ -4913,7 +4936,7 @@
       <c r="BD33" s="31"/>
       <c r="BE33" s="35"/>
     </row>
-    <row r="34" spans="1:57" ht="17" customHeight="1">
+    <row r="34" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
@@ -4972,7 +4995,7 @@
       <c r="BD34" s="33"/>
       <c r="BE34" s="33"/>
     </row>
-    <row r="35" spans="1:57" ht="17" customHeight="1">
+    <row r="35" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="34"/>
       <c r="C35" s="31"/>
@@ -5031,7 +5054,7 @@
       <c r="BD35" s="31"/>
       <c r="BE35" s="35"/>
     </row>
-    <row r="36" spans="1:57" ht="17" customHeight="1">
+    <row r="36" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="32"/>
       <c r="C36" s="33"/>
@@ -5090,7 +5113,7 @@
       <c r="BD36" s="33"/>
       <c r="BE36" s="33"/>
     </row>
-    <row r="37" spans="1:57" ht="17" customHeight="1">
+    <row r="37" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="34"/>
       <c r="C37" s="31"/>
@@ -5149,7 +5172,7 @@
       <c r="BD37" s="31"/>
       <c r="BE37" s="35"/>
     </row>
-    <row r="38" spans="1:57" ht="17" customHeight="1">
+    <row r="38" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="32"/>
       <c r="C38" s="33"/>
@@ -5208,7 +5231,7 @@
       <c r="BD38" s="33"/>
       <c r="BE38" s="33"/>
     </row>
-    <row r="39" spans="1:57" ht="17" customHeight="1">
+    <row r="39" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
       <c r="B39" s="34"/>
       <c r="C39" s="31"/>
@@ -5267,7 +5290,7 @@
       <c r="BD39" s="31"/>
       <c r="BE39" s="35"/>
     </row>
-    <row r="40" spans="1:57" ht="17" customHeight="1">
+    <row r="40" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19"/>
       <c r="B40" s="32"/>
       <c r="C40" s="33"/>
@@ -5326,7 +5349,7 @@
       <c r="BD40" s="33"/>
       <c r="BE40" s="33"/>
     </row>
-    <row r="41" spans="1:57" ht="17" customHeight="1">
+    <row r="41" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="34"/>
       <c r="C41" s="31"/>
@@ -5385,7 +5408,7 @@
       <c r="BD41" s="31"/>
       <c r="BE41" s="35"/>
     </row>
-    <row r="42" spans="1:57" ht="17" customHeight="1">
+    <row r="42" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="32"/>
       <c r="C42" s="33"/>
@@ -5444,7 +5467,7 @@
       <c r="BD42" s="33"/>
       <c r="BE42" s="33"/>
     </row>
-    <row r="43" spans="1:57" ht="17" customHeight="1">
+    <row r="43" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="34"/>
       <c r="C43" s="31"/>
@@ -5503,7 +5526,7 @@
       <c r="BD43" s="31"/>
       <c r="BE43" s="35"/>
     </row>
-    <row r="44" spans="1:57" ht="17" customHeight="1">
+    <row r="44" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="32"/>
       <c r="C44" s="33"/>
@@ -5562,7 +5585,7 @@
       <c r="BD44" s="33"/>
       <c r="BE44" s="33"/>
     </row>
-    <row r="45" spans="1:57" ht="17" customHeight="1">
+    <row r="45" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="34"/>
       <c r="C45" s="31"/>
@@ -5621,7 +5644,7 @@
       <c r="BD45" s="31"/>
       <c r="BE45" s="35"/>
     </row>
-    <row r="46" spans="1:57" ht="17" customHeight="1">
+    <row r="46" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="32"/>
       <c r="C46" s="33"/>
@@ -5680,7 +5703,7 @@
       <c r="BD46" s="33"/>
       <c r="BE46" s="33"/>
     </row>
-    <row r="47" spans="1:57" ht="17" customHeight="1">
+    <row r="47" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="34"/>
       <c r="C47" s="31"/>
@@ -5739,7 +5762,7 @@
       <c r="BD47" s="31"/>
       <c r="BE47" s="35"/>
     </row>
-    <row r="48" spans="1:57" ht="17" customHeight="1">
+    <row r="48" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="32"/>
       <c r="C48" s="33"/>
@@ -5798,7 +5821,7 @@
       <c r="BD48" s="33"/>
       <c r="BE48" s="33"/>
     </row>
-    <row r="49" spans="1:57" ht="17" customHeight="1">
+    <row r="49" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="34"/>
       <c r="C49" s="31"/>
@@ -5857,7 +5880,7 @@
       <c r="BD49" s="31"/>
       <c r="BE49" s="35"/>
     </row>
-    <row r="50" spans="1:57" ht="17" customHeight="1">
+    <row r="50" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="36"/>
       <c r="B50" s="37"/>
       <c r="C50" s="38"/>
@@ -5936,23 +5959,23 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="39" customWidth="1"/>
     <col min="2" max="2" width="48" style="39" customWidth="1"/>
     <col min="3" max="256" width="8.6640625" style="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="43.5" customHeight="1">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="69"/>
+      <c r="B1" s="68"/>
       <c r="C1" s="40"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
     </row>
-    <row r="2" spans="1:5" ht="43.5" customHeight="1">
+    <row r="2" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41"/>
       <c r="B2" s="42" t="s">
         <v>116</v>
@@ -5961,7 +5984,7 @@
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
     </row>
-    <row r="3" spans="1:5" ht="36.75" customHeight="1">
+    <row r="3" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="43" t="s">
         <v>0</v>
       </c>
@@ -5972,7 +5995,7 @@
       <c r="D3" s="29"/>
       <c r="E3" s="29"/>
     </row>
-    <row r="4" spans="1:5" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="45"/>
       <c r="B4" s="18">
         <v>43114</v>
@@ -5981,7 +6004,7 @@
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
     </row>
-    <row r="5" spans="1:5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29"/>
       <c r="B5" s="22">
         <v>43115</v>
@@ -5990,7 +6013,7 @@
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:5" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="22">
         <v>43225</v>
@@ -5999,7 +6022,7 @@
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
     </row>
-    <row r="7" spans="1:5" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29"/>
       <c r="B7" s="22">
         <v>43191</v>
@@ -6008,7 +6031,7 @@
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
     </row>
-    <row r="8" spans="1:5" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
       <c r="B8" s="25" t="s">
         <v>117</v>
@@ -6017,14 +6040,14 @@
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
     </row>
-    <row r="9" spans="1:5" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="29"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
     </row>
-    <row r="10" spans="1:5" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -6047,50 +6070,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV97"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="46" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="46" customWidth="1"/>
     <col min="3" max="3" width="11" style="46" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="46" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="46" customWidth="1"/>
+    <col min="5" max="5" width="23" style="72" customWidth="1"/>
     <col min="6" max="256" width="11" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="60" customHeight="1">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-    </row>
-    <row r="2" spans="1:14" ht="47" customHeight="1">
-      <c r="A2" s="49"/>
-      <c r="B2" s="50" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+    </row>
+    <row r="2" spans="1:14" ht="47" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="48"/>
+      <c r="B2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="51" t="s">
+        <v>122</v>
+      </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
       <c r="H2" s="29"/>
@@ -6101,20 +6126,22 @@
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
     </row>
-    <row r="3" spans="1:14" ht="39" customHeight="1">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="56">
+      <c r="D3" s="55">
         <v>10</v>
       </c>
-      <c r="E3" s="40"/>
+      <c r="E3" s="70">
+        <v>50</v>
+      </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
@@ -6125,18 +6152,20 @@
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A4" s="57"/>
-      <c r="B4" s="58" t="s">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="56"/>
+      <c r="B4" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="59">
         <v>4</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="59">
+        <v>4</v>
+      </c>
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -6147,18 +6176,20 @@
       <c r="M4" s="29"/>
       <c r="N4" s="29"/>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A5" s="61"/>
-      <c r="B5" s="58" t="s">
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="60"/>
+      <c r="B5" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="60">
+      <c r="D5" s="59">
         <v>10</v>
       </c>
-      <c r="E5" s="40"/>
+      <c r="E5" s="59">
+        <v>10</v>
+      </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
       <c r="H5" s="29"/>
@@ -6169,18 +6200,20 @@
       <c r="M5" s="29"/>
       <c r="N5" s="29"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="58" t="s">
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="61"/>
+      <c r="B6" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="59">
         <v>11</v>
       </c>
-      <c r="E6" s="40"/>
+      <c r="E6" s="59">
+        <v>11</v>
+      </c>
       <c r="F6" s="29"/>
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
@@ -6191,18 +6224,20 @@
       <c r="M6" s="29"/>
       <c r="N6" s="29"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A7" s="63"/>
-      <c r="B7" s="58" t="s">
+    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="62"/>
+      <c r="B7" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="59">
         <v>4</v>
       </c>
-      <c r="E7" s="40"/>
+      <c r="E7" s="59">
+        <v>4</v>
+      </c>
       <c r="F7" s="29"/>
       <c r="G7" s="29"/>
       <c r="H7" s="29"/>
@@ -6213,18 +6248,20 @@
       <c r="M7" s="29"/>
       <c r="N7" s="29"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A8" s="63"/>
-      <c r="B8" s="58" t="s">
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62"/>
+      <c r="B8" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="60">
+      <c r="D8" s="59">
         <v>6</v>
       </c>
-      <c r="E8" s="40"/>
+      <c r="E8" s="59">
+        <v>6</v>
+      </c>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
       <c r="H8" s="29"/>
@@ -6235,18 +6272,20 @@
       <c r="M8" s="29"/>
       <c r="N8" s="29"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A9" s="63"/>
-      <c r="B9" s="58" t="s">
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="62"/>
+      <c r="B9" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="59">
         <v>3</v>
       </c>
-      <c r="E9" s="40"/>
+      <c r="E9" s="59">
+        <v>3</v>
+      </c>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
@@ -6257,18 +6296,20 @@
       <c r="M9" s="29"/>
       <c r="N9" s="29"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A10" s="63"/>
-      <c r="B10" s="58" t="s">
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="62"/>
+      <c r="B10" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="59">
         <v>1</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="59">
+        <v>1</v>
+      </c>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
       <c r="H10" s="29"/>
@@ -6279,18 +6320,20 @@
       <c r="M10" s="29"/>
       <c r="N10" s="29"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A11" s="63"/>
-      <c r="B11" s="58" t="s">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="62"/>
+      <c r="B11" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="59">
         <v>6</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="59">
+        <v>6</v>
+      </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
@@ -6301,18 +6344,20 @@
       <c r="M11" s="29"/>
       <c r="N11" s="29"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A12" s="63"/>
-      <c r="B12" s="58" t="s">
+    <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="62"/>
+      <c r="B12" s="57" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="59">
         <v>8</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="59">
+        <v>8</v>
+      </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
@@ -6323,18 +6368,20 @@
       <c r="M12" s="29"/>
       <c r="N12" s="29"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A13" s="63"/>
-      <c r="B13" s="58" t="s">
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="62"/>
+      <c r="B13" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="60">
+      <c r="D13" s="59">
         <v>9</v>
       </c>
-      <c r="E13" s="40"/>
+      <c r="E13" s="59">
+        <v>9</v>
+      </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
@@ -6345,18 +6392,20 @@
       <c r="M13" s="29"/>
       <c r="N13" s="29"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A14" s="63"/>
-      <c r="B14" s="58" t="s">
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="62"/>
+      <c r="B14" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="60">
+      <c r="D14" s="59">
         <v>5</v>
       </c>
-      <c r="E14" s="40"/>
+      <c r="E14" s="59">
+        <v>5</v>
+      </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
@@ -6367,18 +6416,20 @@
       <c r="M14" s="29"/>
       <c r="N14" s="29"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A15" s="63"/>
-      <c r="B15" s="58" t="s">
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="62"/>
+      <c r="B15" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="59" t="s">
+      <c r="C15" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="60">
+      <c r="D15" s="59">
         <v>4</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="59">
+        <v>4</v>
+      </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -6389,18 +6440,20 @@
       <c r="M15" s="29"/>
       <c r="N15" s="29"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A16" s="63"/>
-      <c r="B16" s="58" t="s">
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="62"/>
+      <c r="B16" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="59" t="s">
+      <c r="C16" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="60">
+      <c r="D16" s="59">
         <v>2</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="59">
+        <v>2</v>
+      </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
@@ -6411,18 +6464,20 @@
       <c r="M16" s="29"/>
       <c r="N16" s="29"/>
     </row>
-    <row r="17" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A17" s="63"/>
-      <c r="B17" s="58" t="s">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="62"/>
+      <c r="B17" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="60">
+      <c r="D17" s="59">
         <v>5</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="59">
+        <v>5</v>
+      </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
@@ -6433,18 +6488,20 @@
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
     </row>
-    <row r="18" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A18" s="63"/>
-      <c r="B18" s="58" t="s">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="62"/>
+      <c r="B18" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="59">
         <v>7</v>
       </c>
-      <c r="E18" s="40"/>
+      <c r="E18" s="59">
+        <v>7</v>
+      </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="29"/>
@@ -6455,18 +6512,20 @@
       <c r="M18" s="29"/>
       <c r="N18" s="29"/>
     </row>
-    <row r="19" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A19" s="63"/>
-      <c r="B19" s="58" t="s">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="62"/>
+      <c r="B19" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="59" t="s">
+      <c r="C19" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="60">
+      <c r="D19" s="59">
         <v>15</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="59">
+        <v>15</v>
+      </c>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="29"/>
@@ -6477,18 +6536,20 @@
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
     </row>
-    <row r="20" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="58" t="s">
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="62"/>
+      <c r="B20" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="59">
         <v>3</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="59">
+        <v>3</v>
+      </c>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="29"/>
@@ -6499,18 +6560,20 @@
       <c r="M20" s="29"/>
       <c r="N20" s="29"/>
     </row>
-    <row r="21" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A21" s="63"/>
-      <c r="B21" s="58" t="s">
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="62"/>
+      <c r="B21" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="59" t="s">
+      <c r="C21" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="60">
+      <c r="D21" s="59">
         <v>7</v>
       </c>
-      <c r="E21" s="40"/>
+      <c r="E21" s="59">
+        <v>7</v>
+      </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
@@ -6521,18 +6584,20 @@
       <c r="M21" s="29"/>
       <c r="N21" s="29"/>
     </row>
-    <row r="22" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="58" t="s">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="62"/>
+      <c r="B22" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="59" t="s">
+      <c r="C22" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="60">
+      <c r="D22" s="59">
         <v>0</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="59">
+        <v>0</v>
+      </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
@@ -6543,18 +6608,20 @@
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
     </row>
-    <row r="23" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="58" t="s">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="62"/>
+      <c r="B23" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="60">
+      <c r="D23" s="59">
         <v>3</v>
       </c>
-      <c r="E23" s="40"/>
+      <c r="E23" s="59">
+        <v>3</v>
+      </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
@@ -6565,18 +6632,20 @@
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
     </row>
-    <row r="24" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="B24" s="58" t="s">
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="62"/>
+      <c r="B24" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="59" t="s">
+      <c r="C24" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="D24" s="60">
+      <c r="D24" s="59">
         <v>7</v>
       </c>
-      <c r="E24" s="40"/>
+      <c r="E24" s="59">
+        <v>7</v>
+      </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
@@ -6587,18 +6656,20 @@
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A25" s="63"/>
-      <c r="B25" s="58" t="s">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="62"/>
+      <c r="B25" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="59" t="s">
+      <c r="C25" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="60">
+      <c r="D25" s="59">
         <v>3</v>
       </c>
-      <c r="E25" s="40"/>
+      <c r="E25" s="59">
+        <v>3</v>
+      </c>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
@@ -6609,18 +6680,20 @@
       <c r="M25" s="29"/>
       <c r="N25" s="29"/>
     </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="B26" s="58" t="s">
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="62"/>
+      <c r="B26" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="60">
+      <c r="D26" s="59">
         <v>2</v>
       </c>
-      <c r="E26" s="40"/>
+      <c r="E26" s="59">
+        <v>2</v>
+      </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
@@ -6631,18 +6704,20 @@
       <c r="M26" s="29"/>
       <c r="N26" s="29"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="58" t="s">
+    <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="62"/>
+      <c r="B27" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="59" t="s">
+      <c r="C27" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="60">
+      <c r="D27" s="59">
         <v>5</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="59">
+        <v>5</v>
+      </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
@@ -6653,18 +6728,20 @@
       <c r="M27" s="29"/>
       <c r="N27" s="29"/>
     </row>
-    <row r="28" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="B28" s="58" t="s">
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="62"/>
+      <c r="B28" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="60">
+      <c r="D28" s="59">
         <v>7</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="59">
+        <v>7</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
@@ -6675,18 +6752,20 @@
       <c r="M28" s="29"/>
       <c r="N28" s="29"/>
     </row>
-    <row r="29" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A29" s="63"/>
-      <c r="B29" s="58" t="s">
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="62"/>
+      <c r="B29" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="59" t="s">
+      <c r="C29" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="60">
+      <c r="D29" s="59">
         <v>4</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="59">
+        <v>4</v>
+      </c>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
@@ -6697,18 +6776,20 @@
       <c r="M29" s="29"/>
       <c r="N29" s="29"/>
     </row>
-    <row r="30" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="B30" s="58" t="s">
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="62"/>
+      <c r="B30" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C30" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="60">
+      <c r="D30" s="59">
         <v>4</v>
       </c>
-      <c r="E30" s="40"/>
+      <c r="E30" s="59">
+        <v>4</v>
+      </c>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
@@ -6719,18 +6800,20 @@
       <c r="M30" s="29"/>
       <c r="N30" s="29"/>
     </row>
-    <row r="31" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A31" s="63"/>
-      <c r="B31" s="58" t="s">
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="62"/>
+      <c r="B31" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="60">
+      <c r="D31" s="59">
         <v>2</v>
       </c>
-      <c r="E31" s="40"/>
+      <c r="E31" s="59">
+        <v>2</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
@@ -6741,18 +6824,20 @@
       <c r="M31" s="29"/>
       <c r="N31" s="29"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="B32" s="58" t="s">
+    <row r="32" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="62"/>
+      <c r="B32" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="60">
+      <c r="D32" s="59">
         <v>5</v>
       </c>
-      <c r="E32" s="40"/>
+      <c r="E32" s="59">
+        <v>5</v>
+      </c>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
@@ -6763,18 +6848,20 @@
       <c r="M32" s="29"/>
       <c r="N32" s="29"/>
     </row>
-    <row r="33" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A33" s="63"/>
-      <c r="B33" s="58" t="s">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="62"/>
+      <c r="B33" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="60">
+      <c r="D33" s="59">
         <v>7</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" s="59">
+        <v>7</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
@@ -6785,18 +6872,20 @@
       <c r="M33" s="29"/>
       <c r="N33" s="29"/>
     </row>
-    <row r="34" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="B34" s="58" t="s">
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="62"/>
+      <c r="B34" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="60">
+      <c r="D34" s="59">
         <v>9</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="59">
+        <v>9</v>
+      </c>
       <c r="F34" s="29"/>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
@@ -6807,18 +6896,20 @@
       <c r="M34" s="29"/>
       <c r="N34" s="29"/>
     </row>
-    <row r="35" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A35" s="63"/>
-      <c r="B35" s="58" t="s">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="62"/>
+      <c r="B35" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="60">
+      <c r="D35" s="59">
         <v>4</v>
       </c>
-      <c r="E35" s="40"/>
+      <c r="E35" s="59">
+        <v>4</v>
+      </c>
       <c r="F35" s="29"/>
       <c r="G35" s="29"/>
       <c r="H35" s="29"/>
@@ -6829,18 +6920,20 @@
       <c r="M35" s="29"/>
       <c r="N35" s="29"/>
     </row>
-    <row r="36" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A36" s="63"/>
-      <c r="B36" s="58" t="s">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="62"/>
+      <c r="B36" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="59" t="s">
+      <c r="C36" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="60">
+      <c r="D36" s="59">
         <v>2</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" s="59">
+        <v>2</v>
+      </c>
       <c r="F36" s="29"/>
       <c r="G36" s="29"/>
       <c r="H36" s="29"/>
@@ -6851,18 +6944,20 @@
       <c r="M36" s="29"/>
       <c r="N36" s="29"/>
     </row>
-    <row r="37" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A37" s="63"/>
-      <c r="B37" s="58" t="s">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="62"/>
+      <c r="B37" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="60">
+      <c r="D37" s="59">
         <v>6</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" s="59">
+        <v>6</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="29"/>
       <c r="H37" s="29"/>
@@ -6873,18 +6968,20 @@
       <c r="M37" s="29"/>
       <c r="N37" s="29"/>
     </row>
-    <row r="38" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A38" s="63"/>
-      <c r="B38" s="58" t="s">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="62"/>
+      <c r="B38" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="59" t="s">
+      <c r="C38" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="60">
+      <c r="D38" s="59">
         <v>3</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="59">
+        <v>3</v>
+      </c>
       <c r="F38" s="29"/>
       <c r="G38" s="29"/>
       <c r="H38" s="29"/>
@@ -6895,18 +6992,20 @@
       <c r="M38" s="29"/>
       <c r="N38" s="29"/>
     </row>
-    <row r="39" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A39" s="63"/>
-      <c r="B39" s="58" t="s">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="62"/>
+      <c r="B39" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="59" t="s">
+      <c r="C39" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="60">
+      <c r="D39" s="59">
         <v>2</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="59">
+        <v>2</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
@@ -6917,18 +7016,20 @@
       <c r="M39" s="29"/>
       <c r="N39" s="29"/>
     </row>
-    <row r="40" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A40" s="63"/>
-      <c r="B40" s="58" t="s">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="62"/>
+      <c r="B40" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C40" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="60">
+      <c r="D40" s="59">
         <v>6</v>
       </c>
-      <c r="E40" s="40"/>
+      <c r="E40" s="59">
+        <v>6</v>
+      </c>
       <c r="F40" s="29"/>
       <c r="G40" s="29"/>
       <c r="H40" s="29"/>
@@ -6939,18 +7040,20 @@
       <c r="M40" s="29"/>
       <c r="N40" s="29"/>
     </row>
-    <row r="41" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A41" s="63"/>
-      <c r="B41" s="58" t="s">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="62"/>
+      <c r="B41" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="59" t="s">
+      <c r="C41" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D41" s="60">
+      <c r="D41" s="59">
         <v>5</v>
       </c>
-      <c r="E41" s="40"/>
+      <c r="E41" s="59">
+        <v>5</v>
+      </c>
       <c r="F41" s="29"/>
       <c r="G41" s="29"/>
       <c r="H41" s="29"/>
@@ -6961,18 +7064,20 @@
       <c r="M41" s="29"/>
       <c r="N41" s="29"/>
     </row>
-    <row r="42" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A42" s="63"/>
-      <c r="B42" s="58" t="s">
+    <row r="42" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="62"/>
+      <c r="B42" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="59" t="s">
+      <c r="C42" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="D42" s="60">
+      <c r="D42" s="59">
         <v>3</v>
       </c>
-      <c r="E42" s="40"/>
+      <c r="E42" s="59">
+        <v>3</v>
+      </c>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
       <c r="H42" s="29"/>
@@ -6983,18 +7088,20 @@
       <c r="M42" s="29"/>
       <c r="N42" s="29"/>
     </row>
-    <row r="43" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A43" s="63"/>
-      <c r="B43" s="58" t="s">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="62"/>
+      <c r="B43" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="60">
+      <c r="D43" s="59">
         <v>5</v>
       </c>
-      <c r="E43" s="40"/>
+      <c r="E43" s="59">
+        <v>5</v>
+      </c>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
       <c r="H43" s="29"/>
@@ -7005,18 +7112,20 @@
       <c r="M43" s="29"/>
       <c r="N43" s="29"/>
     </row>
-    <row r="44" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A44" s="63"/>
-      <c r="B44" s="58" t="s">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="62"/>
+      <c r="B44" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="D44" s="60">
+      <c r="D44" s="59">
         <v>36</v>
       </c>
-      <c r="E44" s="40"/>
+      <c r="E44" s="59">
+        <v>36</v>
+      </c>
       <c r="F44" s="29"/>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
@@ -7027,18 +7136,20 @@
       <c r="M44" s="29"/>
       <c r="N44" s="29"/>
     </row>
-    <row r="45" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A45" s="63"/>
-      <c r="B45" s="58" t="s">
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="62"/>
+      <c r="B45" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="D45" s="60">
+      <c r="D45" s="59">
         <v>7</v>
       </c>
-      <c r="E45" s="40"/>
+      <c r="E45" s="59">
+        <v>7</v>
+      </c>
       <c r="F45" s="29"/>
       <c r="G45" s="29"/>
       <c r="H45" s="29"/>
@@ -7049,18 +7160,20 @@
       <c r="M45" s="29"/>
       <c r="N45" s="29"/>
     </row>
-    <row r="46" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A46" s="63"/>
-      <c r="B46" s="58" t="s">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="62"/>
+      <c r="B46" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="60">
+      <c r="D46" s="59">
         <v>1</v>
       </c>
-      <c r="E46" s="40"/>
+      <c r="E46" s="59">
+        <v>1</v>
+      </c>
       <c r="F46" s="29"/>
       <c r="G46" s="29"/>
       <c r="H46" s="29"/>
@@ -7071,18 +7184,20 @@
       <c r="M46" s="29"/>
       <c r="N46" s="29"/>
     </row>
-    <row r="47" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A47" s="63"/>
-      <c r="B47" s="58" t="s">
+    <row r="47" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="62"/>
+      <c r="B47" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="59" t="s">
+      <c r="C47" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="60">
+      <c r="D47" s="59">
         <v>4</v>
       </c>
-      <c r="E47" s="40"/>
+      <c r="E47" s="59">
+        <v>4</v>
+      </c>
       <c r="F47" s="29"/>
       <c r="G47" s="29"/>
       <c r="H47" s="29"/>
@@ -7093,18 +7208,20 @@
       <c r="M47" s="29"/>
       <c r="N47" s="29"/>
     </row>
-    <row r="48" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A48" s="63"/>
-      <c r="B48" s="58" t="s">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="62"/>
+      <c r="B48" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="C48" s="59" t="s">
+      <c r="C48" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D48" s="60">
+      <c r="D48" s="59">
         <v>57</v>
       </c>
-      <c r="E48" s="40"/>
+      <c r="E48" s="59">
+        <v>57</v>
+      </c>
       <c r="F48" s="29"/>
       <c r="G48" s="29"/>
       <c r="H48" s="29"/>
@@ -7115,18 +7232,20 @@
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
     </row>
-    <row r="49" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A49" s="63"/>
-      <c r="B49" s="58" t="s">
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="62"/>
+      <c r="B49" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="C49" s="59" t="s">
+      <c r="C49" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="D49" s="60">
+      <c r="D49" s="59">
         <v>3</v>
       </c>
-      <c r="E49" s="40"/>
+      <c r="E49" s="59">
+        <v>3</v>
+      </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
       <c r="H49" s="29"/>
@@ -7137,18 +7256,20 @@
       <c r="M49" s="29"/>
       <c r="N49" s="29"/>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A50" s="63"/>
-      <c r="B50" s="58" t="s">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="62"/>
+      <c r="B50" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="59" t="s">
+      <c r="C50" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="60">
+      <c r="D50" s="59">
         <v>1</v>
       </c>
-      <c r="E50" s="40"/>
+      <c r="E50" s="59">
+        <v>1</v>
+      </c>
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
       <c r="H50" s="29"/>
@@ -7159,18 +7280,20 @@
       <c r="M50" s="29"/>
       <c r="N50" s="29"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A51" s="63"/>
-      <c r="B51" s="58" t="s">
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="62"/>
+      <c r="B51" s="57" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="60">
+      <c r="D51" s="59">
         <v>7</v>
       </c>
-      <c r="E51" s="40"/>
+      <c r="E51" s="59">
+        <v>7</v>
+      </c>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
       <c r="H51" s="29"/>
@@ -7181,18 +7304,20 @@
       <c r="M51" s="29"/>
       <c r="N51" s="29"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A52" s="63"/>
-      <c r="B52" s="58" t="s">
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="62"/>
+      <c r="B52" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="59" t="s">
+      <c r="C52" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="60">
+      <c r="D52" s="59">
         <v>4</v>
       </c>
-      <c r="E52" s="40"/>
+      <c r="E52" s="59">
+        <v>4</v>
+      </c>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
       <c r="H52" s="29"/>
@@ -7203,18 +7328,20 @@
       <c r="M52" s="29"/>
       <c r="N52" s="29"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A53" s="63"/>
-      <c r="B53" s="58" t="s">
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="62"/>
+      <c r="B53" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="C53" s="59" t="s">
+      <c r="C53" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="D53" s="60">
+      <c r="D53" s="59">
         <v>2</v>
       </c>
-      <c r="E53" s="40"/>
+      <c r="E53" s="59">
+        <v>2</v>
+      </c>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
       <c r="H53" s="29"/>
@@ -7225,18 +7352,20 @@
       <c r="M53" s="29"/>
       <c r="N53" s="29"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A54" s="63"/>
-      <c r="B54" s="58" t="s">
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="62"/>
+      <c r="B54" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="59" t="s">
+      <c r="C54" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="60">
+      <c r="D54" s="59">
         <v>6</v>
       </c>
-      <c r="E54" s="40"/>
+      <c r="E54" s="59">
+        <v>6</v>
+      </c>
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
       <c r="H54" s="29"/>
@@ -7247,18 +7376,20 @@
       <c r="M54" s="29"/>
       <c r="N54" s="29"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A55" s="63"/>
-      <c r="B55" s="58" t="s">
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="62"/>
+      <c r="B55" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="C55" s="59" t="s">
+      <c r="C55" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="60">
+      <c r="D55" s="59">
         <v>2</v>
       </c>
-      <c r="E55" s="40"/>
+      <c r="E55" s="59">
+        <v>2</v>
+      </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
       <c r="H55" s="29"/>
@@ -7269,18 +7400,20 @@
       <c r="M55" s="29"/>
       <c r="N55" s="29"/>
     </row>
-    <row r="56" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A56" s="63"/>
-      <c r="B56" s="58" t="s">
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="62"/>
+      <c r="B56" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="C56" s="59" t="s">
+      <c r="C56" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="D56" s="60">
+      <c r="D56" s="59">
         <v>2</v>
       </c>
-      <c r="E56" s="40"/>
+      <c r="E56" s="59">
+        <v>2</v>
+      </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
       <c r="H56" s="29"/>
@@ -7291,18 +7424,20 @@
       <c r="M56" s="29"/>
       <c r="N56" s="29"/>
     </row>
-    <row r="57" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A57" s="63"/>
-      <c r="B57" s="58" t="s">
+    <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="62"/>
+      <c r="B57" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="59" t="s">
+      <c r="C57" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="D57" s="60">
+      <c r="D57" s="59">
         <v>6</v>
       </c>
-      <c r="E57" s="40"/>
+      <c r="E57" s="59">
+        <v>6</v>
+      </c>
       <c r="F57" s="29"/>
       <c r="G57" s="29"/>
       <c r="H57" s="29"/>
@@ -7313,18 +7448,20 @@
       <c r="M57" s="29"/>
       <c r="N57" s="29"/>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A58" s="63"/>
-      <c r="B58" s="58" t="s">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="62"/>
+      <c r="B58" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="59" t="s">
+      <c r="C58" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="D58" s="60">
+      <c r="D58" s="59">
         <v>1</v>
       </c>
-      <c r="E58" s="40"/>
+      <c r="E58" s="59">
+        <v>1</v>
+      </c>
       <c r="F58" s="29"/>
       <c r="G58" s="29"/>
       <c r="H58" s="29"/>
@@ -7335,12 +7472,12 @@
       <c r="M58" s="29"/>
       <c r="N58" s="29"/>
     </row>
-    <row r="59" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A59" s="63"/>
-      <c r="B59" s="64"/>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="62"/>
+      <c r="B59" s="63"/>
       <c r="C59" s="29"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="40"/>
+      <c r="D59" s="59"/>
+      <c r="E59" s="71"/>
       <c r="F59" s="29"/>
       <c r="G59" s="29"/>
       <c r="H59" s="29"/>
@@ -7351,12 +7488,12 @@
       <c r="M59" s="29"/>
       <c r="N59" s="29"/>
     </row>
-    <row r="60" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A60" s="63"/>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="62"/>
       <c r="B60" s="40"/>
       <c r="C60" s="29"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="40"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="71"/>
       <c r="F60" s="29"/>
       <c r="G60" s="29"/>
       <c r="H60" s="29"/>
@@ -7367,12 +7504,12 @@
       <c r="M60" s="29"/>
       <c r="N60" s="29"/>
     </row>
-    <row r="61" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A61" s="63"/>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="62"/>
       <c r="B61" s="40"/>
       <c r="C61" s="29"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="40"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="71"/>
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
@@ -7383,12 +7520,12 @@
       <c r="M61" s="29"/>
       <c r="N61" s="29"/>
     </row>
-    <row r="62" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A62" s="63"/>
+    <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="62"/>
       <c r="B62" s="40"/>
       <c r="C62" s="29"/>
-      <c r="D62" s="60"/>
-      <c r="E62" s="40"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="71"/>
       <c r="F62" s="29"/>
       <c r="G62" s="29"/>
       <c r="H62" s="29"/>
@@ -7399,12 +7536,12 @@
       <c r="M62" s="29"/>
       <c r="N62" s="29"/>
     </row>
-    <row r="63" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A63" s="63"/>
+    <row r="63" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="62"/>
       <c r="B63" s="40"/>
       <c r="C63" s="29"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="40"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="71"/>
       <c r="F63" s="29"/>
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
@@ -7415,12 +7552,12 @@
       <c r="M63" s="29"/>
       <c r="N63" s="29"/>
     </row>
-    <row r="64" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A64" s="63"/>
+    <row r="64" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="62"/>
       <c r="B64" s="40"/>
       <c r="C64" s="29"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="40"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="71"/>
       <c r="F64" s="29"/>
       <c r="G64" s="29"/>
       <c r="H64" s="29"/>
@@ -7431,12 +7568,12 @@
       <c r="M64" s="29"/>
       <c r="N64" s="29"/>
     </row>
-    <row r="65" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A65" s="63"/>
+    <row r="65" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="62"/>
       <c r="B65" s="40"/>
       <c r="C65" s="29"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="40"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="71"/>
       <c r="F65" s="29"/>
       <c r="G65" s="29"/>
       <c r="H65" s="29"/>
@@ -7447,12 +7584,12 @@
       <c r="M65" s="29"/>
       <c r="N65" s="29"/>
     </row>
-    <row r="66" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A66" s="63"/>
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="62"/>
       <c r="B66" s="40"/>
       <c r="C66" s="29"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="40"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="71"/>
       <c r="F66" s="29"/>
       <c r="G66" s="29"/>
       <c r="H66" s="29"/>
@@ -7463,12 +7600,12 @@
       <c r="M66" s="29"/>
       <c r="N66" s="29"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A67" s="63"/>
+    <row r="67" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="62"/>
       <c r="B67" s="40"/>
       <c r="C67" s="29"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="40"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="71"/>
       <c r="F67" s="29"/>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
@@ -7479,12 +7616,12 @@
       <c r="M67" s="29"/>
       <c r="N67" s="29"/>
     </row>
-    <row r="68" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A68" s="63"/>
+    <row r="68" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="62"/>
       <c r="B68" s="40"/>
       <c r="C68" s="29"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="40"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="71"/>
       <c r="F68" s="29"/>
       <c r="G68" s="29"/>
       <c r="H68" s="29"/>
@@ -7495,12 +7632,12 @@
       <c r="M68" s="29"/>
       <c r="N68" s="29"/>
     </row>
-    <row r="69" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A69" s="63"/>
+    <row r="69" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="62"/>
       <c r="B69" s="40"/>
       <c r="C69" s="29"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="40"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="71"/>
       <c r="F69" s="29"/>
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
@@ -7511,12 +7648,12 @@
       <c r="M69" s="29"/>
       <c r="N69" s="29"/>
     </row>
-    <row r="70" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A70" s="63"/>
+    <row r="70" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="62"/>
       <c r="B70" s="40"/>
       <c r="C70" s="29"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="40"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="71"/>
       <c r="F70" s="29"/>
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
@@ -7527,12 +7664,12 @@
       <c r="M70" s="29"/>
       <c r="N70" s="29"/>
     </row>
-    <row r="71" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A71" s="63"/>
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="62"/>
       <c r="B71" s="40"/>
       <c r="C71" s="29"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="40"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="71"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
@@ -7543,12 +7680,12 @@
       <c r="M71" s="29"/>
       <c r="N71" s="29"/>
     </row>
-    <row r="72" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A72" s="63"/>
+    <row r="72" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="62"/>
       <c r="B72" s="40"/>
       <c r="C72" s="29"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="40"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="71"/>
       <c r="F72" s="29"/>
       <c r="G72" s="29"/>
       <c r="H72" s="29"/>
@@ -7559,12 +7696,12 @@
       <c r="M72" s="29"/>
       <c r="N72" s="29"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A73" s="63"/>
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="62"/>
       <c r="B73" s="40"/>
       <c r="C73" s="29"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="40"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="71"/>
       <c r="F73" s="29"/>
       <c r="G73" s="29"/>
       <c r="H73" s="29"/>
@@ -7575,12 +7712,12 @@
       <c r="M73" s="29"/>
       <c r="N73" s="29"/>
     </row>
-    <row r="74" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A74" s="63"/>
+    <row r="74" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="62"/>
       <c r="B74" s="40"/>
       <c r="C74" s="29"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="40"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="71"/>
       <c r="F74" s="29"/>
       <c r="G74" s="29"/>
       <c r="H74" s="29"/>
@@ -7591,12 +7728,12 @@
       <c r="M74" s="29"/>
       <c r="N74" s="29"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A75" s="63"/>
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="62"/>
       <c r="B75" s="40"/>
       <c r="C75" s="29"/>
-      <c r="D75" s="60"/>
-      <c r="E75" s="40"/>
+      <c r="D75" s="59"/>
+      <c r="E75" s="71"/>
       <c r="F75" s="29"/>
       <c r="G75" s="29"/>
       <c r="H75" s="29"/>
@@ -7607,12 +7744,12 @@
       <c r="M75" s="29"/>
       <c r="N75" s="29"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A76" s="63"/>
+    <row r="76" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="62"/>
       <c r="B76" s="40"/>
       <c r="C76" s="29"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="40"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="71"/>
       <c r="F76" s="29"/>
       <c r="G76" s="29"/>
       <c r="H76" s="29"/>
@@ -7623,12 +7760,12 @@
       <c r="M76" s="29"/>
       <c r="N76" s="29"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A77" s="63"/>
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="62"/>
       <c r="B77" s="40"/>
       <c r="C77" s="29"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="40"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="71"/>
       <c r="F77" s="29"/>
       <c r="G77" s="29"/>
       <c r="H77" s="29"/>
@@ -7639,12 +7776,12 @@
       <c r="M77" s="29"/>
       <c r="N77" s="29"/>
     </row>
-    <row r="78" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A78" s="63"/>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="62"/>
       <c r="B78" s="40"/>
       <c r="C78" s="29"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="40"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="71"/>
       <c r="F78" s="29"/>
       <c r="G78" s="29"/>
       <c r="H78" s="29"/>
@@ -7655,12 +7792,12 @@
       <c r="M78" s="29"/>
       <c r="N78" s="29"/>
     </row>
-    <row r="79" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A79" s="63"/>
+    <row r="79" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="62"/>
       <c r="B79" s="40"/>
       <c r="C79" s="29"/>
-      <c r="D79" s="60"/>
-      <c r="E79" s="40"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="71"/>
       <c r="F79" s="29"/>
       <c r="G79" s="29"/>
       <c r="H79" s="29"/>
@@ -7671,12 +7808,12 @@
       <c r="M79" s="29"/>
       <c r="N79" s="29"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A80" s="63"/>
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="62"/>
       <c r="B80" s="40"/>
       <c r="C80" s="29"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="40"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="71"/>
       <c r="F80" s="29"/>
       <c r="G80" s="29"/>
       <c r="H80" s="29"/>
@@ -7687,12 +7824,12 @@
       <c r="M80" s="29"/>
       <c r="N80" s="29"/>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A81" s="63"/>
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="62"/>
       <c r="B81" s="40"/>
       <c r="C81" s="29"/>
-      <c r="D81" s="60"/>
-      <c r="E81" s="40"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="71"/>
       <c r="F81" s="29"/>
       <c r="G81" s="29"/>
       <c r="H81" s="29"/>
@@ -7703,12 +7840,12 @@
       <c r="M81" s="29"/>
       <c r="N81" s="29"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A82" s="63"/>
+    <row r="82" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="62"/>
       <c r="B82" s="40"/>
       <c r="C82" s="29"/>
-      <c r="D82" s="60"/>
-      <c r="E82" s="40"/>
+      <c r="D82" s="59"/>
+      <c r="E82" s="71"/>
       <c r="F82" s="29"/>
       <c r="G82" s="29"/>
       <c r="H82" s="29"/>
@@ -7719,12 +7856,12 @@
       <c r="M82" s="29"/>
       <c r="N82" s="29"/>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A83" s="63"/>
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="62"/>
       <c r="B83" s="40"/>
       <c r="C83" s="29"/>
-      <c r="D83" s="60"/>
-      <c r="E83" s="40"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="71"/>
       <c r="F83" s="29"/>
       <c r="G83" s="29"/>
       <c r="H83" s="29"/>
@@ -7735,12 +7872,12 @@
       <c r="M83" s="29"/>
       <c r="N83" s="29"/>
     </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A84" s="63"/>
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="62"/>
       <c r="B84" s="40"/>
       <c r="C84" s="29"/>
-      <c r="D84" s="60"/>
-      <c r="E84" s="40"/>
+      <c r="D84" s="59"/>
+      <c r="E84" s="71"/>
       <c r="F84" s="29"/>
       <c r="G84" s="29"/>
       <c r="H84" s="29"/>
@@ -7751,12 +7888,12 @@
       <c r="M84" s="29"/>
       <c r="N84" s="29"/>
     </row>
-    <row r="85" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A85" s="63"/>
+    <row r="85" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="62"/>
       <c r="B85" s="40"/>
       <c r="C85" s="29"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="40"/>
+      <c r="D85" s="59"/>
+      <c r="E85" s="71"/>
       <c r="F85" s="29"/>
       <c r="G85" s="29"/>
       <c r="H85" s="29"/>
@@ -7767,12 +7904,12 @@
       <c r="M85" s="29"/>
       <c r="N85" s="29"/>
     </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A86" s="63"/>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="62"/>
       <c r="B86" s="40"/>
       <c r="C86" s="29"/>
-      <c r="D86" s="60"/>
-      <c r="E86" s="40"/>
+      <c r="D86" s="59"/>
+      <c r="E86" s="71"/>
       <c r="F86" s="29"/>
       <c r="G86" s="29"/>
       <c r="H86" s="29"/>
@@ -7783,12 +7920,12 @@
       <c r="M86" s="29"/>
       <c r="N86" s="29"/>
     </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A87" s="63"/>
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="62"/>
       <c r="B87" s="40"/>
       <c r="C87" s="29"/>
-      <c r="D87" s="60"/>
-      <c r="E87" s="40"/>
+      <c r="D87" s="59"/>
+      <c r="E87" s="71"/>
       <c r="F87" s="29"/>
       <c r="G87" s="29"/>
       <c r="H87" s="29"/>
@@ -7799,12 +7936,12 @@
       <c r="M87" s="29"/>
       <c r="N87" s="29"/>
     </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A88" s="63"/>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="62"/>
       <c r="B88" s="40"/>
       <c r="C88" s="29"/>
-      <c r="D88" s="60"/>
-      <c r="E88" s="40"/>
+      <c r="D88" s="59"/>
+      <c r="E88" s="71"/>
       <c r="F88" s="29"/>
       <c r="G88" s="29"/>
       <c r="H88" s="29"/>
@@ -7815,12 +7952,12 @@
       <c r="M88" s="29"/>
       <c r="N88" s="29"/>
     </row>
-    <row r="89" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A89" s="63"/>
+    <row r="89" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="62"/>
       <c r="B89" s="40"/>
       <c r="C89" s="29"/>
-      <c r="D89" s="60"/>
-      <c r="E89" s="40"/>
+      <c r="D89" s="59"/>
+      <c r="E89" s="71"/>
       <c r="F89" s="29"/>
       <c r="G89" s="29"/>
       <c r="H89" s="29"/>
@@ -7831,12 +7968,12 @@
       <c r="M89" s="29"/>
       <c r="N89" s="29"/>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A90" s="63"/>
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="62"/>
       <c r="B90" s="40"/>
       <c r="C90" s="29"/>
-      <c r="D90" s="60"/>
-      <c r="E90" s="40"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="71"/>
       <c r="F90" s="29"/>
       <c r="G90" s="29"/>
       <c r="H90" s="29"/>
@@ -7847,12 +7984,12 @@
       <c r="M90" s="29"/>
       <c r="N90" s="29"/>
     </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A91" s="63"/>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="62"/>
       <c r="B91" s="40"/>
       <c r="C91" s="29"/>
-      <c r="D91" s="60"/>
-      <c r="E91" s="40"/>
+      <c r="D91" s="59"/>
+      <c r="E91" s="71"/>
       <c r="F91" s="29"/>
       <c r="G91" s="29"/>
       <c r="H91" s="29"/>
@@ -7863,12 +8000,12 @@
       <c r="M91" s="29"/>
       <c r="N91" s="29"/>
     </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A92" s="63"/>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="62"/>
       <c r="B92" s="40"/>
       <c r="C92" s="29"/>
-      <c r="D92" s="60"/>
-      <c r="E92" s="40"/>
+      <c r="D92" s="59"/>
+      <c r="E92" s="71"/>
       <c r="F92" s="29"/>
       <c r="G92" s="29"/>
       <c r="H92" s="29"/>
@@ -7879,12 +8016,12 @@
       <c r="M92" s="29"/>
       <c r="N92" s="29"/>
     </row>
-    <row r="93" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A93" s="63"/>
+    <row r="93" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="62"/>
       <c r="B93" s="40"/>
       <c r="C93" s="29"/>
-      <c r="D93" s="60"/>
-      <c r="E93" s="40"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="71"/>
       <c r="F93" s="29"/>
       <c r="G93" s="29"/>
       <c r="H93" s="29"/>
@@ -7895,12 +8032,12 @@
       <c r="M93" s="29"/>
       <c r="N93" s="29"/>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A94" s="63"/>
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="62"/>
       <c r="B94" s="40"/>
       <c r="C94" s="29"/>
-      <c r="D94" s="60"/>
-      <c r="E94" s="40"/>
+      <c r="D94" s="59"/>
+      <c r="E94" s="71"/>
       <c r="F94" s="29"/>
       <c r="G94" s="29"/>
       <c r="H94" s="29"/>
@@ -7911,12 +8048,12 @@
       <c r="M94" s="29"/>
       <c r="N94" s="29"/>
     </row>
-    <row r="95" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A95" s="63"/>
+    <row r="95" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="62"/>
       <c r="B95" s="40"/>
       <c r="C95" s="29"/>
-      <c r="D95" s="60"/>
-      <c r="E95" s="40"/>
+      <c r="D95" s="59"/>
+      <c r="E95" s="71"/>
       <c r="F95" s="29"/>
       <c r="G95" s="29"/>
       <c r="H95" s="29"/>
@@ -7927,12 +8064,12 @@
       <c r="M95" s="29"/>
       <c r="N95" s="29"/>
     </row>
-    <row r="96" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A96" s="63"/>
+    <row r="96" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="62"/>
       <c r="B96" s="40"/>
       <c r="C96" s="29"/>
-      <c r="D96" s="60"/>
-      <c r="E96" s="40"/>
+      <c r="D96" s="59"/>
+      <c r="E96" s="71"/>
       <c r="F96" s="29"/>
       <c r="G96" s="29"/>
       <c r="H96" s="29"/>
@@ -7943,12 +8080,12 @@
       <c r="M96" s="29"/>
       <c r="N96" s="29"/>
     </row>
-    <row r="97" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A97" s="65"/>
+    <row r="97" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="64"/>
       <c r="B97" s="40"/>
       <c r="C97" s="29"/>
-      <c r="D97" s="60"/>
-      <c r="E97" s="40"/>
+      <c r="D97" s="59"/>
+      <c r="E97" s="71"/>
       <c r="F97" s="29"/>
       <c r="G97" s="29"/>
       <c r="H97" s="29"/>
@@ -7961,7 +8098,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
small cosmetic spreadsheet fixes
</commit_message>
<xml_diff>
--- a/spec/support/validRoSpreadsheet.xlsx
+++ b/spec/support/validRoSpreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenhalliburton/workspace/caseflow/spec/support/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navaloaner_2/workspace/caseflow/spec/support/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF95FDD3-10D1-3749-BD00-E8A4203A0C81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEA354B-0008-3340-9C81-DD16D7F58975}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3460" yWindow="800" windowWidth="37280" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId1"/>
@@ -384,13 +384,13 @@
     <t>Allocation of Regional Office Video Hearings</t>
   </si>
   <si>
-    <t>Number of Hearing Days Allocated in Date Range</t>
-  </si>
-  <si>
     <t xml:space="preserve">Des Moines, IA </t>
   </si>
   <si>
     <t>Number of Hearing Days Without Rooms in Date Range</t>
+  </si>
+  <si>
+    <t>Number of Hearing Days with 425 I Rooms Allocated in Date Range</t>
   </si>
 </sst>
 </file>
@@ -1074,6 +1074,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1089,9 +1092,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2290,9 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IT50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2310,19 +2308,19 @@
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -5967,10 +5965,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="71"/>
       <c r="C1" s="40"/>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
@@ -6070,8 +6068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IV97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6080,12 +6078,12 @@
     <col min="2" max="2" width="23.5" style="46" customWidth="1"/>
     <col min="3" max="3" width="11" style="46" customWidth="1"/>
     <col min="4" max="4" width="22.5" style="46" customWidth="1"/>
-    <col min="5" max="5" width="23" style="72" customWidth="1"/>
+    <col min="5" max="5" width="23" style="67" customWidth="1"/>
     <col min="6" max="256" width="11" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="72" t="s">
         <v>119</v>
       </c>
       <c r="B1" s="73"/>
@@ -6111,10 +6109,10 @@
         <v>2</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E2" s="51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -6139,7 +6137,7 @@
       <c r="D3" s="55">
         <v>10</v>
       </c>
-      <c r="E3" s="70">
+      <c r="E3" s="65">
         <v>50</v>
       </c>
       <c r="F3" s="29"/>
@@ -6803,7 +6801,7 @@
     <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="62"/>
       <c r="B31" s="57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C31" s="58" t="s">
         <v>31</v>
@@ -7477,7 +7475,7 @@
       <c r="B59" s="63"/>
       <c r="C59" s="29"/>
       <c r="D59" s="59"/>
-      <c r="E59" s="71"/>
+      <c r="E59" s="66"/>
       <c r="F59" s="29"/>
       <c r="G59" s="29"/>
       <c r="H59" s="29"/>
@@ -7493,7 +7491,7 @@
       <c r="B60" s="40"/>
       <c r="C60" s="29"/>
       <c r="D60" s="59"/>
-      <c r="E60" s="71"/>
+      <c r="E60" s="66"/>
       <c r="F60" s="29"/>
       <c r="G60" s="29"/>
       <c r="H60" s="29"/>
@@ -7509,7 +7507,7 @@
       <c r="B61" s="40"/>
       <c r="C61" s="29"/>
       <c r="D61" s="59"/>
-      <c r="E61" s="71"/>
+      <c r="E61" s="66"/>
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
       <c r="H61" s="29"/>
@@ -7525,7 +7523,7 @@
       <c r="B62" s="40"/>
       <c r="C62" s="29"/>
       <c r="D62" s="59"/>
-      <c r="E62" s="71"/>
+      <c r="E62" s="66"/>
       <c r="F62" s="29"/>
       <c r="G62" s="29"/>
       <c r="H62" s="29"/>
@@ -7541,7 +7539,7 @@
       <c r="B63" s="40"/>
       <c r="C63" s="29"/>
       <c r="D63" s="59"/>
-      <c r="E63" s="71"/>
+      <c r="E63" s="66"/>
       <c r="F63" s="29"/>
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
@@ -7557,7 +7555,7 @@
       <c r="B64" s="40"/>
       <c r="C64" s="29"/>
       <c r="D64" s="59"/>
-      <c r="E64" s="71"/>
+      <c r="E64" s="66"/>
       <c r="F64" s="29"/>
       <c r="G64" s="29"/>
       <c r="H64" s="29"/>
@@ -7573,7 +7571,7 @@
       <c r="B65" s="40"/>
       <c r="C65" s="29"/>
       <c r="D65" s="59"/>
-      <c r="E65" s="71"/>
+      <c r="E65" s="66"/>
       <c r="F65" s="29"/>
       <c r="G65" s="29"/>
       <c r="H65" s="29"/>
@@ -7589,7 +7587,7 @@
       <c r="B66" s="40"/>
       <c r="C66" s="29"/>
       <c r="D66" s="59"/>
-      <c r="E66" s="71"/>
+      <c r="E66" s="66"/>
       <c r="F66" s="29"/>
       <c r="G66" s="29"/>
       <c r="H66" s="29"/>
@@ -7605,7 +7603,7 @@
       <c r="B67" s="40"/>
       <c r="C67" s="29"/>
       <c r="D67" s="59"/>
-      <c r="E67" s="71"/>
+      <c r="E67" s="66"/>
       <c r="F67" s="29"/>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
@@ -7621,7 +7619,7 @@
       <c r="B68" s="40"/>
       <c r="C68" s="29"/>
       <c r="D68" s="59"/>
-      <c r="E68" s="71"/>
+      <c r="E68" s="66"/>
       <c r="F68" s="29"/>
       <c r="G68" s="29"/>
       <c r="H68" s="29"/>
@@ -7637,7 +7635,7 @@
       <c r="B69" s="40"/>
       <c r="C69" s="29"/>
       <c r="D69" s="59"/>
-      <c r="E69" s="71"/>
+      <c r="E69" s="66"/>
       <c r="F69" s="29"/>
       <c r="G69" s="29"/>
       <c r="H69" s="29"/>
@@ -7653,7 +7651,7 @@
       <c r="B70" s="40"/>
       <c r="C70" s="29"/>
       <c r="D70" s="59"/>
-      <c r="E70" s="71"/>
+      <c r="E70" s="66"/>
       <c r="F70" s="29"/>
       <c r="G70" s="29"/>
       <c r="H70" s="29"/>
@@ -7669,7 +7667,7 @@
       <c r="B71" s="40"/>
       <c r="C71" s="29"/>
       <c r="D71" s="59"/>
-      <c r="E71" s="71"/>
+      <c r="E71" s="66"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29"/>
       <c r="H71" s="29"/>
@@ -7685,7 +7683,7 @@
       <c r="B72" s="40"/>
       <c r="C72" s="29"/>
       <c r="D72" s="59"/>
-      <c r="E72" s="71"/>
+      <c r="E72" s="66"/>
       <c r="F72" s="29"/>
       <c r="G72" s="29"/>
       <c r="H72" s="29"/>
@@ -7701,7 +7699,7 @@
       <c r="B73" s="40"/>
       <c r="C73" s="29"/>
       <c r="D73" s="59"/>
-      <c r="E73" s="71"/>
+      <c r="E73" s="66"/>
       <c r="F73" s="29"/>
       <c r="G73" s="29"/>
       <c r="H73" s="29"/>
@@ -7717,7 +7715,7 @@
       <c r="B74" s="40"/>
       <c r="C74" s="29"/>
       <c r="D74" s="59"/>
-      <c r="E74" s="71"/>
+      <c r="E74" s="66"/>
       <c r="F74" s="29"/>
       <c r="G74" s="29"/>
       <c r="H74" s="29"/>
@@ -7733,7 +7731,7 @@
       <c r="B75" s="40"/>
       <c r="C75" s="29"/>
       <c r="D75" s="59"/>
-      <c r="E75" s="71"/>
+      <c r="E75" s="66"/>
       <c r="F75" s="29"/>
       <c r="G75" s="29"/>
       <c r="H75" s="29"/>
@@ -7749,7 +7747,7 @@
       <c r="B76" s="40"/>
       <c r="C76" s="29"/>
       <c r="D76" s="59"/>
-      <c r="E76" s="71"/>
+      <c r="E76" s="66"/>
       <c r="F76" s="29"/>
       <c r="G76" s="29"/>
       <c r="H76" s="29"/>
@@ -7765,7 +7763,7 @@
       <c r="B77" s="40"/>
       <c r="C77" s="29"/>
       <c r="D77" s="59"/>
-      <c r="E77" s="71"/>
+      <c r="E77" s="66"/>
       <c r="F77" s="29"/>
       <c r="G77" s="29"/>
       <c r="H77" s="29"/>
@@ -7781,7 +7779,7 @@
       <c r="B78" s="40"/>
       <c r="C78" s="29"/>
       <c r="D78" s="59"/>
-      <c r="E78" s="71"/>
+      <c r="E78" s="66"/>
       <c r="F78" s="29"/>
       <c r="G78" s="29"/>
       <c r="H78" s="29"/>
@@ -7797,7 +7795,7 @@
       <c r="B79" s="40"/>
       <c r="C79" s="29"/>
       <c r="D79" s="59"/>
-      <c r="E79" s="71"/>
+      <c r="E79" s="66"/>
       <c r="F79" s="29"/>
       <c r="G79" s="29"/>
       <c r="H79" s="29"/>
@@ -7813,7 +7811,7 @@
       <c r="B80" s="40"/>
       <c r="C80" s="29"/>
       <c r="D80" s="59"/>
-      <c r="E80" s="71"/>
+      <c r="E80" s="66"/>
       <c r="F80" s="29"/>
       <c r="G80" s="29"/>
       <c r="H80" s="29"/>
@@ -7829,7 +7827,7 @@
       <c r="B81" s="40"/>
       <c r="C81" s="29"/>
       <c r="D81" s="59"/>
-      <c r="E81" s="71"/>
+      <c r="E81" s="66"/>
       <c r="F81" s="29"/>
       <c r="G81" s="29"/>
       <c r="H81" s="29"/>
@@ -7845,7 +7843,7 @@
       <c r="B82" s="40"/>
       <c r="C82" s="29"/>
       <c r="D82" s="59"/>
-      <c r="E82" s="71"/>
+      <c r="E82" s="66"/>
       <c r="F82" s="29"/>
       <c r="G82" s="29"/>
       <c r="H82" s="29"/>
@@ -7861,7 +7859,7 @@
       <c r="B83" s="40"/>
       <c r="C83" s="29"/>
       <c r="D83" s="59"/>
-      <c r="E83" s="71"/>
+      <c r="E83" s="66"/>
       <c r="F83" s="29"/>
       <c r="G83" s="29"/>
       <c r="H83" s="29"/>
@@ -7877,7 +7875,7 @@
       <c r="B84" s="40"/>
       <c r="C84" s="29"/>
       <c r="D84" s="59"/>
-      <c r="E84" s="71"/>
+      <c r="E84" s="66"/>
       <c r="F84" s="29"/>
       <c r="G84" s="29"/>
       <c r="H84" s="29"/>
@@ -7893,7 +7891,7 @@
       <c r="B85" s="40"/>
       <c r="C85" s="29"/>
       <c r="D85" s="59"/>
-      <c r="E85" s="71"/>
+      <c r="E85" s="66"/>
       <c r="F85" s="29"/>
       <c r="G85" s="29"/>
       <c r="H85" s="29"/>
@@ -7909,7 +7907,7 @@
       <c r="B86" s="40"/>
       <c r="C86" s="29"/>
       <c r="D86" s="59"/>
-      <c r="E86" s="71"/>
+      <c r="E86" s="66"/>
       <c r="F86" s="29"/>
       <c r="G86" s="29"/>
       <c r="H86" s="29"/>
@@ -7925,7 +7923,7 @@
       <c r="B87" s="40"/>
       <c r="C87" s="29"/>
       <c r="D87" s="59"/>
-      <c r="E87" s="71"/>
+      <c r="E87" s="66"/>
       <c r="F87" s="29"/>
       <c r="G87" s="29"/>
       <c r="H87" s="29"/>
@@ -7941,7 +7939,7 @@
       <c r="B88" s="40"/>
       <c r="C88" s="29"/>
       <c r="D88" s="59"/>
-      <c r="E88" s="71"/>
+      <c r="E88" s="66"/>
       <c r="F88" s="29"/>
       <c r="G88" s="29"/>
       <c r="H88" s="29"/>
@@ -7957,7 +7955,7 @@
       <c r="B89" s="40"/>
       <c r="C89" s="29"/>
       <c r="D89" s="59"/>
-      <c r="E89" s="71"/>
+      <c r="E89" s="66"/>
       <c r="F89" s="29"/>
       <c r="G89" s="29"/>
       <c r="H89" s="29"/>
@@ -7973,7 +7971,7 @@
       <c r="B90" s="40"/>
       <c r="C90" s="29"/>
       <c r="D90" s="59"/>
-      <c r="E90" s="71"/>
+      <c r="E90" s="66"/>
       <c r="F90" s="29"/>
       <c r="G90" s="29"/>
       <c r="H90" s="29"/>
@@ -7989,7 +7987,7 @@
       <c r="B91" s="40"/>
       <c r="C91" s="29"/>
       <c r="D91" s="59"/>
-      <c r="E91" s="71"/>
+      <c r="E91" s="66"/>
       <c r="F91" s="29"/>
       <c r="G91" s="29"/>
       <c r="H91" s="29"/>
@@ -8005,7 +8003,7 @@
       <c r="B92" s="40"/>
       <c r="C92" s="29"/>
       <c r="D92" s="59"/>
-      <c r="E92" s="71"/>
+      <c r="E92" s="66"/>
       <c r="F92" s="29"/>
       <c r="G92" s="29"/>
       <c r="H92" s="29"/>
@@ -8021,7 +8019,7 @@
       <c r="B93" s="40"/>
       <c r="C93" s="29"/>
       <c r="D93" s="59"/>
-      <c r="E93" s="71"/>
+      <c r="E93" s="66"/>
       <c r="F93" s="29"/>
       <c r="G93" s="29"/>
       <c r="H93" s="29"/>
@@ -8037,7 +8035,7 @@
       <c r="B94" s="40"/>
       <c r="C94" s="29"/>
       <c r="D94" s="59"/>
-      <c r="E94" s="71"/>
+      <c r="E94" s="66"/>
       <c r="F94" s="29"/>
       <c r="G94" s="29"/>
       <c r="H94" s="29"/>
@@ -8053,7 +8051,7 @@
       <c r="B95" s="40"/>
       <c r="C95" s="29"/>
       <c r="D95" s="59"/>
-      <c r="E95" s="71"/>
+      <c r="E95" s="66"/>
       <c r="F95" s="29"/>
       <c r="G95" s="29"/>
       <c r="H95" s="29"/>
@@ -8069,7 +8067,7 @@
       <c r="B96" s="40"/>
       <c r="C96" s="29"/>
       <c r="D96" s="59"/>
-      <c r="E96" s="71"/>
+      <c r="E96" s="66"/>
       <c r="F96" s="29"/>
       <c r="G96" s="29"/>
       <c r="H96" s="29"/>
@@ -8085,7 +8083,7 @@
       <c r="B97" s="40"/>
       <c r="C97" s="29"/>
       <c r="D97" s="59"/>
-      <c r="E97" s="71"/>
+      <c r="E97" s="66"/>
       <c r="F97" s="29"/>
       <c r="G97" s="29"/>
       <c r="H97" s="29"/>

</xml_diff>